<commit_message>
Ampliacion cambio contraseña y planificador tareas modificado.
</commit_message>
<xml_diff>
--- a/Planificador de Tareas.xlsx
+++ b/Planificador de Tareas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carde\Desktop\ISW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CEU\4º Curso\ISW\OCR\ISW\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1A65ADA-1633-436E-B99E-90E7F1865E8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B34F535B-AD0C-446A-B6E4-38F40F8585B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D1E1BE30-6AFF-4741-A4AD-A6F9DB8F2C33}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{D1E1BE30-6AFF-4741-A4AD-A6F9DB8F2C33}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
   <si>
     <t>REQUISITO 23: Registro de usuario</t>
   </si>
@@ -56,12 +56,15 @@
     <t>TIEMPO(min)</t>
   </si>
   <si>
+    <t>Video Tutoriales/formación Python</t>
+  </si>
+  <si>
+    <t>Miguel</t>
+  </si>
+  <si>
     <t>Video Tutoriales</t>
   </si>
   <si>
-    <t>Miguel</t>
-  </si>
-  <si>
     <t>Juan Pablo</t>
   </si>
   <si>
@@ -86,9 +89,6 @@
     <t>Funcionamiento conjunto Inicio-Registro</t>
   </si>
   <si>
-    <t>(AMBOS)</t>
-  </si>
-  <si>
     <t>Funcionamiento conjunto</t>
   </si>
   <si>
@@ -101,13 +101,16 @@
     <t>REQUISITO 25: Cambiar Contraseña</t>
   </si>
   <si>
-    <t>Miguel y Juan Pablo</t>
-  </si>
-  <si>
     <t>Búsqueda Información Cambio Contraseña</t>
   </si>
   <si>
-    <t>Video Tutoriales/formación Python</t>
+    <t xml:space="preserve">Integración </t>
+  </si>
+  <si>
+    <t>Desarrollo Código Introducir Nueva Contraseña</t>
+  </si>
+  <si>
+    <t>Desarrollo Código Requisitos Cambio Contraseña</t>
   </si>
 </sst>
 </file>
@@ -316,6 +319,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -325,9 +331,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -346,10 +349,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -649,15 +648,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0B2028-F346-4B99-9600-D486646BEA8E}">
-  <dimension ref="B1:H17"/>
+  <dimension ref="B1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.5703125" customWidth="1"/>
     <col min="5" max="5" width="12.28515625" customWidth="1"/>
@@ -668,19 +667,19 @@
   <sheetData>
     <row r="1" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
       <c r="E2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="10"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="13"/>
     </row>
     <row r="3" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
@@ -707,7 +706,7 @@
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -716,10 +715,10 @@
         <v>60</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H4" s="2">
         <v>60</v>
@@ -727,19 +726,19 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="2">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H5" s="2">
         <v>20</v>
@@ -747,19 +746,19 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="2">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H6" s="2">
         <v>5</v>
@@ -767,7 +766,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
         <v>7</v>
@@ -776,10 +775,10 @@
         <v>20</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H7" s="2">
         <v>20</v>
@@ -787,19 +786,19 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="D8" s="2">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H8" s="2">
         <v>45</v>
@@ -807,26 +806,22 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="2"/>
+      <c r="E9">
         <v>30</v>
-      </c>
-      <c r="E9" t="s">
-        <v>16</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="G9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" s="2">
-        <v>30</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
@@ -842,7 +837,7 @@
         <v>18</v>
       </c>
       <c r="G10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H10" s="2">
         <v>5</v>
@@ -855,11 +850,11 @@
       <c r="C11" s="4"/>
       <c r="D11" s="5">
         <f>D4+D5+D6+D8+D7+D9+D10</f>
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="E11" s="4">
-        <f>D11+H11</f>
-        <v>350</v>
+        <f>D11+H11+E9</f>
+        <v>349</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>19</v>
@@ -867,57 +862,102 @@
       <c r="G11" s="4"/>
       <c r="H11" s="5">
         <f>SUM(H4:H10)</f>
-        <v>185</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="12"/>
       <c r="D13" s="14"/>
     </row>
     <row r="14" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D15" s="2">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="D16" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="3" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18" s="2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="2">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5">
-        <v>25</v>
+      <c r="C21" s="4"/>
+      <c r="D21" s="5">
+        <f>D15+D16+D19+D17+D20+D18</f>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
@@ -1212,14 +1252,14 @@
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD0FFF94-1A5D-4FF5-A525-0D12D1F8F370}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a136fbf0-cb94-4dcb-bf5d-fe776b794717"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="222120fa-f9ef-48bb-8261-756bcdc1f761"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="222120fa-f9ef-48bb-8261-756bcdc1f761"/>
-    <ds:schemaRef ds:uri="a136fbf0-cb94-4dcb-bf5d-fe776b794717"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>

</xml_diff>

<commit_message>
inicio de la interfaz gráfica
</commit_message>
<xml_diff>
--- a/Planificador de Tareas.xlsx
+++ b/Planificador de Tareas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Carlosramos_0/Desktop/ISW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5A6B84F-B908-0A40-9ADB-468D092028A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A681CA8-C23A-474A-B2E0-6F6777E598AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14260" xr2:uid="{D1E1BE30-6AFF-4741-A4AD-A6F9DB8F2C33}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{D1E1BE30-6AFF-4741-A4AD-A6F9DB8F2C33}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="39">
   <si>
     <t>REQUISITO 23: Registro de usuario</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>Instalación e investigación  de paquetes</t>
+  </si>
+  <si>
+    <t>total</t>
   </si>
 </sst>
 </file>
@@ -184,7 +187,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="25">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -352,28 +355,6 @@
       <left style="medium">
         <color rgb="FF000000"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -395,19 +376,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -462,13 +430,37 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -478,7 +470,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -488,6 +480,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -500,19 +500,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -829,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0B2028-F346-4B99-9600-D486646BEA8E}">
   <dimension ref="B1:M31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="G6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -848,17 +839,17 @@
   <sheetData>
     <row r="1" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="10" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="11"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="19"/>
     </row>
     <row r="3" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -870,7 +861,7 @@
       <c r="D3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G3" s="4" t="s">
@@ -959,16 +950,16 @@
       <c r="H7" s="2">
         <v>20</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="K7" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="L7" s="22" t="s">
+      <c r="L7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="M7" s="21" t="s">
+      <c r="M7" s="13" t="s">
         <v>35</v>
       </c>
     </row>
@@ -994,13 +985,13 @@
       <c r="J8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="23" t="s">
+      <c r="K8" s="15" t="s">
         <v>5</v>
       </c>
       <c r="L8" s="2">
         <v>60</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="11">
         <v>30</v>
       </c>
     </row>
@@ -1026,13 +1017,13 @@
       <c r="J9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K9" s="24" t="s">
+      <c r="K9" s="16" t="s">
         <v>5</v>
       </c>
       <c r="L9" s="2">
         <v>24</v>
       </c>
-      <c r="M9" s="18">
+      <c r="M9" s="12">
         <v>25</v>
       </c>
     </row>
@@ -1058,13 +1049,13 @@
       <c r="J10" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K10" s="24" t="s">
+      <c r="K10" s="16" t="s">
         <v>5</v>
       </c>
       <c r="L10" s="2">
         <v>20</v>
       </c>
-      <c r="M10" s="18">
+      <c r="M10" s="12">
         <v>20</v>
       </c>
     </row>
@@ -1077,7 +1068,7 @@
         <f>D4+D5+D6+D8+D7+D9+D10</f>
         <v>194</v>
       </c>
-      <c r="E11" s="13"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="4" t="s">
         <v>17</v>
       </c>
@@ -1089,13 +1080,13 @@
       <c r="J11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K11" s="24" t="s">
+      <c r="K11" s="16" t="s">
         <v>5</v>
       </c>
       <c r="L11" s="2">
         <v>20</v>
       </c>
-      <c r="M11" s="18">
+      <c r="M11" s="12">
         <v>35</v>
       </c>
     </row>
@@ -1103,37 +1094,37 @@
       <c r="J12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="K12" s="24" t="s">
+      <c r="K12" s="16" t="s">
         <v>5</v>
       </c>
       <c r="L12" s="2">
         <v>35</v>
       </c>
-      <c r="M12" s="18">
+      <c r="M12" s="12">
         <v>30</v>
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="9" t="s">
+      <c r="B13" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="12"/>
-      <c r="F13" s="9" t="s">
+      <c r="C13" s="18"/>
+      <c r="D13" s="20"/>
+      <c r="F13" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="12"/>
+      <c r="G13" s="18"/>
+      <c r="H13" s="20"/>
       <c r="J13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K13" s="24" t="s">
+      <c r="K13" s="16" t="s">
         <v>5</v>
       </c>
       <c r="L13" s="2">
         <v>30</v>
       </c>
-      <c r="M13" s="18">
+      <c r="M13" s="12">
         <v>20</v>
       </c>
     </row>
@@ -1159,13 +1150,13 @@
       <c r="J14" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K14" s="24" t="s">
+      <c r="K14" s="16" t="s">
         <v>5</v>
       </c>
       <c r="L14" s="2">
         <v>1</v>
       </c>
-      <c r="M14" s="18">
+      <c r="M14" s="12">
         <v>1</v>
       </c>
     </row>
@@ -1191,13 +1182,13 @@
       <c r="J15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K15" s="24" t="s">
+      <c r="K15" s="16" t="s">
         <v>5</v>
       </c>
       <c r="L15" s="2">
         <v>20</v>
       </c>
-      <c r="M15" s="18">
+      <c r="M15" s="12">
         <v>15</v>
       </c>
     </row>
@@ -1223,13 +1214,13 @@
       <c r="J16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K16" s="24" t="s">
+      <c r="K16" s="16" t="s">
         <v>7</v>
       </c>
       <c r="L16" s="2">
         <v>5</v>
       </c>
-      <c r="M16" s="18">
+      <c r="M16" s="12">
         <v>20</v>
       </c>
     </row>
@@ -1255,13 +1246,13 @@
       <c r="J17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="K17" s="24" t="s">
+      <c r="K17" s="16" t="s">
         <v>7</v>
       </c>
       <c r="L17" s="2">
         <v>30</v>
       </c>
-      <c r="M17" s="18">
+      <c r="M17" s="12">
         <v>20</v>
       </c>
     </row>
@@ -1285,13 +1276,13 @@
       <c r="J18" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K18" s="24" t="s">
+      <c r="K18" s="16" t="s">
         <v>7</v>
       </c>
       <c r="L18" s="2">
         <v>13</v>
       </c>
-      <c r="M18" s="18">
+      <c r="M18" s="12">
         <v>10</v>
       </c>
     </row>
@@ -1308,13 +1299,13 @@
       <c r="J19" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="K19" s="24" t="s">
+      <c r="K19" s="16" t="s">
         <v>5</v>
       </c>
       <c r="L19" s="2">
         <v>20</v>
       </c>
-      <c r="M19" s="18">
+      <c r="M19" s="12">
         <v>20</v>
       </c>
     </row>
@@ -1331,13 +1322,13 @@
       <c r="J20" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="K20" s="24" t="s">
+      <c r="K20" s="16" t="s">
         <v>7</v>
       </c>
       <c r="L20" s="2">
         <v>55</v>
       </c>
-      <c r="M20" s="18">
+      <c r="M20" s="12">
         <v>45</v>
       </c>
     </row>
@@ -1353,13 +1344,13 @@
       <c r="J21" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K21" s="24" t="s">
+      <c r="K21" s="16" t="s">
         <v>7</v>
       </c>
       <c r="L21" s="2">
         <v>60</v>
       </c>
-      <c r="M21" s="18">
+      <c r="M21" s="12">
         <v>40</v>
       </c>
     </row>
@@ -1367,13 +1358,13 @@
       <c r="J22" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K22" s="24" t="s">
+      <c r="K22" s="16" t="s">
         <v>7</v>
       </c>
       <c r="L22" s="2">
         <v>20</v>
       </c>
-      <c r="M22" s="18">
+      <c r="M22" s="12">
         <v>15</v>
       </c>
     </row>
@@ -1381,13 +1372,13 @@
       <c r="J23" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K23" s="24" t="s">
+      <c r="K23" s="16" t="s">
         <v>7</v>
       </c>
       <c r="L23" s="2">
         <v>5</v>
       </c>
-      <c r="M23" s="18">
+      <c r="M23" s="12">
         <v>3</v>
       </c>
     </row>
@@ -1395,13 +1386,13 @@
       <c r="J24" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K24" s="24" t="s">
+      <c r="K24" s="16" t="s">
         <v>7</v>
       </c>
       <c r="L24" s="2">
         <v>20</v>
       </c>
-      <c r="M24" s="18">
+      <c r="M24" s="12">
         <v>10</v>
       </c>
     </row>
@@ -1409,13 +1400,13 @@
       <c r="J25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K25" s="24" t="s">
+      <c r="K25" s="16" t="s">
         <v>7</v>
       </c>
       <c r="L25" s="2">
         <v>45</v>
       </c>
-      <c r="M25" s="18">
+      <c r="M25" s="12">
         <v>45</v>
       </c>
     </row>
@@ -1423,13 +1414,13 @@
       <c r="J26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="K26" s="24" t="s">
+      <c r="K26" s="16" t="s">
         <v>7</v>
       </c>
       <c r="L26" s="2">
         <v>30</v>
       </c>
-      <c r="M26" s="18">
+      <c r="M26" s="12">
         <v>30</v>
       </c>
     </row>
@@ -1437,13 +1428,13 @@
       <c r="J27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="K27" s="24" t="s">
+      <c r="K27" s="16" t="s">
         <v>7</v>
       </c>
       <c r="L27" s="2">
         <v>5</v>
       </c>
-      <c r="M27" s="18">
+      <c r="M27" s="12">
         <v>10</v>
       </c>
     </row>
@@ -1451,13 +1442,13 @@
       <c r="J28" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="K28" s="24" t="s">
+      <c r="K28" s="16" t="s">
         <v>26</v>
       </c>
       <c r="L28" s="2">
         <v>120</v>
       </c>
-      <c r="M28" s="18">
+      <c r="M28" s="12">
         <v>90</v>
       </c>
     </row>
@@ -1465,32 +1456,43 @@
       <c r="J29" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="K29" s="24" t="s">
+      <c r="K29" s="16" t="s">
         <v>26</v>
       </c>
       <c r="L29" s="2">
         <v>20</v>
       </c>
-      <c r="M29" s="18">
+      <c r="M29" s="12">
         <v>30</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="J30" s="15" t="s">
+      <c r="J30" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K30" s="25" t="s">
+      <c r="K30" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="L30" s="16">
+      <c r="L30" s="2">
         <v>30</v>
       </c>
-      <c r="M30" s="19">
+      <c r="M30" s="12">
         <v>15</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="M31" s="20"/>
+      <c r="J31" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="K31" s="21"/>
+      <c r="L31" s="22">
+        <f>SUM(L8:L30)</f>
+        <v>688</v>
+      </c>
+      <c r="M31" s="23">
+        <f>SUM(M8:M30)</f>
+        <v>579</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -1504,23 +1506,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="222120fa-f9ef-48bb-8261-756bcdc1f761" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101000C8B8C3005359240A32C95D7972A29AE" ma:contentTypeVersion="15" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="4a2da8c18401be365d12918e652b5702">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="222120fa-f9ef-48bb-8261-756bcdc1f761" xmlns:ns4="a136fbf0-cb94-4dcb-bf5d-fe776b794717" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="880271ac67ff508fa6afb497b6e8fa0e" ns3:_="" ns4:_="">
     <xsd:import namespace="222120fa-f9ef-48bb-8261-756bcdc1f761"/>
@@ -1755,10 +1740,38 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="222120fa-f9ef-48bb-8261-756bcdc1f761" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{714E55DA-D509-457D-A8DE-620BD2901DB5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{581A9279-45A5-4B22-A329-8D25BEB45D64}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="222120fa-f9ef-48bb-8261-756bcdc1f761"/>
+    <ds:schemaRef ds:uri="a136fbf0-cb94-4dcb-bf5d-fe776b794717"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1781,20 +1794,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{581A9279-45A5-4B22-A329-8D25BEB45D64}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{714E55DA-D509-457D-A8DE-620BD2901DB5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="222120fa-f9ef-48bb-8261-756bcdc1f761"/>
-    <ds:schemaRef ds:uri="a136fbf0-cb94-4dcb-bf5d-fe776b794717"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
planificador de tareas actualizado
</commit_message>
<xml_diff>
--- a/Planificador de Tareas.xlsx
+++ b/Planificador de Tareas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Carlosramos_0/Desktop/ISW/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A681CA8-C23A-474A-B2E0-6F6777E598AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4016CE-18C2-B145-87BE-093E7887BF21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{D1E1BE30-6AFF-4741-A4AD-A6F9DB8F2C33}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14300" xr2:uid="{D1E1BE30-6AFF-4741-A4AD-A6F9DB8F2C33}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="42">
   <si>
     <t>REQUISITO 23: Registro de usuario</t>
   </si>
@@ -150,6 +150,15 @@
   </si>
   <si>
     <t>total</t>
+  </si>
+  <si>
+    <t>fracasar con textual</t>
+  </si>
+  <si>
+    <t>video tutorial de textual</t>
+  </si>
+  <si>
+    <t>interfaz grafica texteual</t>
   </si>
 </sst>
 </file>
@@ -470,7 +479,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -488,6 +497,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -500,10 +513,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -818,10 +831,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C0B2028-F346-4B99-9600-D486646BEA8E}">
-  <dimension ref="B1:M31"/>
+  <dimension ref="B1:M36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G6" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="N21" sqref="N21"/>
+    <sheetView tabSelected="1" topLeftCell="F13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -839,17 +852,17 @@
   <sheetData>
     <row r="1" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
       <c r="E2" s="9"/>
-      <c r="F2" s="18" t="s">
+      <c r="F2" s="22" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="18"/>
-      <c r="H2" s="19"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="23"/>
     </row>
     <row r="3" spans="2:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
@@ -1105,16 +1118,16 @@
       </c>
     </row>
     <row r="13" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="17" t="s">
+      <c r="B13" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="18"/>
-      <c r="D13" s="20"/>
-      <c r="F13" s="17" t="s">
+      <c r="C13" s="22"/>
+      <c r="D13" s="24"/>
+      <c r="F13" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="G13" s="18"/>
-      <c r="H13" s="20"/>
+      <c r="G13" s="22"/>
+      <c r="H13" s="24"/>
       <c r="J13" s="1" t="s">
         <v>14</v>
       </c>
@@ -1481,17 +1494,59 @@
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="J31" s="24" t="s">
+      <c r="J31" s="25" t="s">
+        <v>39</v>
+      </c>
+      <c r="K31" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="L31" s="27">
+        <v>120</v>
+      </c>
+      <c r="M31" s="28">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="J32" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="K32" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="L32" s="27">
+        <v>60</v>
+      </c>
+      <c r="M32" s="28">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="10:13" x14ac:dyDescent="0.2">
+      <c r="J33" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="K33" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="L33" s="27">
+        <v>120</v>
+      </c>
+      <c r="M33" s="28">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="36" spans="10:13" x14ac:dyDescent="0.2">
+      <c r="J36" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="K31" s="21"/>
-      <c r="L31" s="22">
-        <f>SUM(L8:L30)</f>
-        <v>688</v>
-      </c>
-      <c r="M31" s="23">
-        <f>SUM(M8:M30)</f>
-        <v>579</v>
+      <c r="K36" s="17"/>
+      <c r="L36" s="18">
+        <f>SUM(L8:L33)</f>
+        <v>988</v>
+      </c>
+      <c r="M36" s="19">
+        <f>SUM(M8:M33)</f>
+        <v>799</v>
       </c>
     </row>
   </sheetData>
@@ -1506,6 +1561,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="222120fa-f9ef-48bb-8261-756bcdc1f761" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101000C8B8C3005359240A32C95D7972A29AE" ma:contentTypeVersion="15" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="4a2da8c18401be365d12918e652b5702">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="222120fa-f9ef-48bb-8261-756bcdc1f761" xmlns:ns4="a136fbf0-cb94-4dcb-bf5d-fe776b794717" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="880271ac67ff508fa6afb497b6e8fa0e" ns3:_="" ns4:_="">
     <xsd:import namespace="222120fa-f9ef-48bb-8261-756bcdc1f761"/>
@@ -1740,14 +1803,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="222120fa-f9ef-48bb-8261-756bcdc1f761" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1758,6 +1813,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD0FFF94-1A5D-4FF5-A525-0D12D1F8F370}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="a136fbf0-cb94-4dcb-bf5d-fe776b794717"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="222120fa-f9ef-48bb-8261-756bcdc1f761"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{581A9279-45A5-4B22-A329-8D25BEB45D64}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1776,23 +1848,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DD0FFF94-1A5D-4FF5-A525-0D12D1F8F370}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="a136fbf0-cb94-4dcb-bf5d-fe776b794717"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="222120fa-f9ef-48bb-8261-756bcdc1f761"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{714E55DA-D509-457D-A8DE-620BD2901DB5}">
   <ds:schemaRefs>

</xml_diff>